<commit_message>
Remove clipped images from the files
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
+++ b/SubRES_TMPL/SubRES_PWR_ElectricityStorage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10FBE42-641C-4773-992D-31B214D70E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094C92C0-F1DC-48EC-BAE1-F5ADC5E21510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>ETRI 2014</t>
-  </si>
-  <si>
-    <t>Which battery Type?</t>
   </si>
   <si>
     <t>ELE,STGTSS</t>
@@ -1245,8 +1242,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1681,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -1770,10 +1767,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
@@ -1802,10 +1799,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
@@ -1834,10 +1831,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -1894,10 +1891,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
@@ -1982,10 +1979,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
@@ -2070,7 +2067,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="24">
         <v>1</v>
@@ -2102,10 +2099,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="30" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>61</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
@@ -2134,10 +2131,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>63</v>
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
@@ -2167,7 +2164,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -4097,8 +4094,8 @@
   </sheetPr>
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4324,43 +4321,41 @@
       <c r="Y4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="AA4" s="10"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="J5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N5" s="4">
         <v>2023</v>
@@ -4403,37 +4398,37 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N6" s="4">
         <v>2023</v>
@@ -4473,37 +4468,37 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="J7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="L7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N7" s="4">
         <v>2023</v>

</xml_diff>